<commit_message>
Updates GRA for carbon tax to fund normal government spending
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D819826-0E41-444E-85CC-5113AD7B4B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D403A752-3D22-40DF-B3A5-473D36DD7D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60480" yWindow="1125" windowWidth="23430" windowHeight="14790" tabRatio="698" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -407,9 +407,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -447,7 +447,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -553,7 +553,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -695,7 +695,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,19 +713,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="80.85546875" customWidth="1"/>
+    <col min="2" max="2" width="80.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -733,72 +735,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -806,7 +808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -814,7 +816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -822,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -830,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -838,114 +840,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -967,12 +969,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -980,7 +982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -989,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -997,7 +999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1005,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1037,12 +1039,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1050,7 +1052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1075,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1105,12 +1107,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1118,7 +1120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1127,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1173,12 +1175,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1186,7 +1188,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1195,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1219,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1239,37 +1241,37 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1279,7 +1281,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1299,27 +1301,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1439,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1489,12 +1491,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1514,32 +1516,32 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="10">
         <f>IFERROR(B8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="10">
         <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1664,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1689,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1754,15 +1756,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1770,40 +1772,40 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1827,12 +1829,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1840,7 +1842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1849,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1873,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1895,12 +1897,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1908,7 +1910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1917,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1965,12 +1967,12 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2011,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2033,12 +2035,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2046,7 +2048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2055,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2063,7 +2065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2079,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2101,12 +2103,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2114,7 +2116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2123,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2131,7 +2133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2147,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2169,12 +2171,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2182,7 +2184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2191,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2207,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2215,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Shifts 25% of ETS income to labor and consumers to account for 50% of ETS 2's going to social fund
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D403A752-3D22-40DF-B3A5-473D36DD7D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C69A18-F6F0-46FC-AA77-800D7DE544E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60480" yWindow="1125" windowWidth="23430" windowHeight="14790" tabRatio="698" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1242,7 +1242,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1306,13 +1306,13 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B22" s="10">
         <f>IFERROR(B8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C22" s="10">
         <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="B2">
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1794,7 +1794,7 @@
         <v>49</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>